<commit_message>
Expand available spectrum types and add interface translation
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="299">
   <si>
     <t>Identifier</t>
   </si>
@@ -920,6 +920,12 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Modified Bretschneider</t>
+  </si>
+  <si>
+    <t>Regular</t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2731,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2767,13 +2773,19 @@
         <v>111</v>
       </c>
       <c r="B2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2" t="s">
         <v>232</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>233</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Started categorisation of site data
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="301">
   <si>
     <t>Identifier</t>
   </si>
@@ -926,6 +926,12 @@
   </si>
   <si>
     <t>Regular</t>
+  </si>
+  <si>
+    <t>Lease Area</t>
+  </si>
+  <si>
+    <t>Wave Resource</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1016,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1033,6 +1039,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1044,12 +1063,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1063,12 +1079,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1083,35 +1094,43 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -1488,901 +1507,919 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.36328125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.6328125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="107.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="1020" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="29"/>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+    <row r="18" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
+    <row r="20" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="24" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
+    <row r="21" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
+    <row r="25" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="E26" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="G26" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19" t="s">
+    <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="E27" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="G27" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="E28" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="G28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="19" t="s">
+    <row r="29" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="24" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="26" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="20" t="s">
+    <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="H31" s="26" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
+    <row r="33" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" s="26" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20" t="s">
+    <row r="34" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="H34" s="15" t="s">
+      <c r="D34" s="27"/>
+      <c r="H34" s="26" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="26" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="20" t="s">
+    <row r="36" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="H37" s="26" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+    <row r="38" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="29"/>
-      <c r="H38" s="15" t="s">
+      <c r="D38" s="27"/>
+      <c r="H38" s="26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="20" t="s">
+    <row r="39" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="H39" s="15" t="s">
+      <c r="H39" s="26" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="20" t="s">
+    <row r="41" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="26" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="19" t="s">
+    <row r="42" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="24" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="19" t="s">
+    <row r="43" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="25" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="20" t="s">
+    <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="27" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="20" t="s">
+    <row r="45" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="D45" s="29"/>
-      <c r="H45" s="15" t="s">
+      <c r="D45" s="27"/>
+      <c r="H45" s="26" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="15" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="20" t="s">
+    <row r="46" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="D46" s="29"/>
-      <c r="H46" s="15" t="s">
+      <c r="D46" s="27"/>
+      <c r="H46" s="26" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="19" t="s">
+    <row r="47" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="28"/>
-      <c r="G47" s="2" t="s">
+      <c r="D47" s="25"/>
+      <c r="G47" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="21" t="s">
+    <row r="48" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="29" t="s">
         <v>185</v>
       </c>
       <c r="D48" s="30" t="s">
         <v>290</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5" t="s">
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="24" t="s">
+      <c r="H48" s="29"/>
+    </row>
+    <row r="49" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="27" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2737,7 +2774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3027,7 +3064,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="8" t="s">
         <v>284</v>
       </c>
       <c r="B23" t="s">
@@ -3044,7 +3081,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B24" t="s">
@@ -3136,16 +3173,16 @@
       <c r="D4" t="s">
         <v>261</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>265</v>
       </c>
     </row>
@@ -3162,16 +3199,16 @@
       <c r="D5" t="s">
         <v>266</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>265</v>
       </c>
     </row>
@@ -3204,36 +3241,36 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
         <v>269</v>
       </c>
     </row>
@@ -3545,7 +3582,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B33" t="s">
@@ -3553,7 +3590,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="10" t="s">
         <v>138</v>
       </c>
       <c r="B34" t="s">
@@ -3561,7 +3598,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B35" t="s">
@@ -3569,7 +3606,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B36" t="s">
@@ -3577,7 +3614,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B37" t="s">
@@ -3585,7 +3622,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B38" t="s">
@@ -3593,7 +3630,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B39" t="s">

</xml_diff>

<commit_message>
Removed farm.point_sea_surface_height as a variable as should always be zero.
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Labels" sheetId="5" r:id="rId5"/>
     <sheet name="Types" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="296">
   <si>
     <t>Identifier</t>
   </si>
@@ -307,18 +307,6 @@
     <t>hydrodynamics: Main_Direction.</t>
   </si>
   <si>
-    <t>farm.point_sea_surface_height</t>
-  </si>
-  <si>
-    <t>Single Point Sea Surface Height</t>
-  </si>
-  <si>
-    <t>Sea surface elevation at a single point within the array.</t>
-  </si>
-  <si>
-    <t>hydrodynamics: MetoceanConditions["SSH"].</t>
-  </si>
-  <si>
     <t>farm.power_law_exponent</t>
   </si>
   <si>
@@ -644,9 +632,6 @@
   </si>
   <si>
     <t>array_main_direction</t>
-  </si>
-  <si>
-    <t>sea_surface_elevation</t>
   </si>
   <si>
     <t>power_law_exponent</t>
@@ -1505,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1538,10 +1523,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>2</v>
@@ -1997,6 +1982,12 @@
       <c r="D25" s="25" t="s">
         <v>102</v>
       </c>
+      <c r="E25" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>290</v>
+      </c>
       <c r="G25" s="24" t="s">
         <v>26</v>
       </c>
@@ -2018,96 +2009,87 @@
         <v>106</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="25" t="s">
-        <v>110</v>
-      </c>
       <c r="E27" s="24" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G27" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="24" t="s">
+      <c r="D28" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="G28" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
+    </row>
+    <row r="29" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>288</v>
-      </c>
-      <c r="C29" s="24" t="s">
+      <c r="B29" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="C29" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="24" t="s">
+      <c r="D29" s="27" t="s">
         <v>117</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>120</v>
@@ -2124,7 +2106,7 @@
         <v>123</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>124</v>
@@ -2141,7 +2123,7 @@
         <v>127</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>128</v>
@@ -2158,29 +2140,29 @@
         <v>131</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="27"/>
+      <c r="H33" s="26" t="s">
         <v>133</v>
-      </c>
-      <c r="H33" s="26" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="26" t="s">
+      <c r="D34" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="27"/>
       <c r="H34" s="26" t="s">
         <v>137</v>
       </c>
@@ -2190,7 +2172,7 @@
         <v>138</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C35" s="26" t="s">
         <v>139</v>
@@ -2198,21 +2180,21 @@
       <c r="D35" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="H35" s="26" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="36" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="D36" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="H36" s="26" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2221,39 +2203,39 @@
         <v>145</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>289</v>
+        <v>115</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="27"/>
+      <c r="H37" s="26" t="s">
         <v>147</v>
-      </c>
-      <c r="H37" s="26" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="26" t="s">
         <v>149</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>119</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="27"/>
+      <c r="D38" s="27" t="s">
+        <v>151</v>
+      </c>
       <c r="H38" s="26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>154</v>
@@ -2261,166 +2243,149 @@
       <c r="D39" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="H39" s="26" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="40" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="D40" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="H40" s="26" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B41" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="26" t="s">
+      <c r="B41" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="C41" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H41" s="26" t="s">
+      <c r="D41" s="25" t="s">
         <v>163</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H42" s="24" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B43" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>172</v>
+      <c r="C43" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
-        <v>279</v>
+        <v>170</v>
       </c>
       <c r="B44" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="H44" s="26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C44" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
+      <c r="B45" s="26" t="s">
         <v>174</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>173</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>175</v>
       </c>
       <c r="D45" s="27"/>
       <c r="H45" s="26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="14" t="s">
+      <c r="B46" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="D46" s="25"/>
+      <c r="G46" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="B47" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="D46" s="27"/>
-      <c r="H46" s="26" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="13" t="s">
+      <c r="C47" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="B47" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D47" s="25"/>
-      <c r="G47" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>285</v>
-      </c>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="H48" s="29"/>
-    </row>
-    <row r="49" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>284</v>
+      <c r="H47" s="29"/>
+    </row>
+    <row r="48" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2431,10 +2396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2454,22 +2419,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2477,10 +2442,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2488,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2499,10 +2464,10 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2510,10 +2475,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -2521,10 +2486,10 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -2532,10 +2497,10 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2543,10 +2508,10 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2554,10 +2519,10 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2565,10 +2530,10 @@
         <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2576,10 +2541,10 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2587,10 +2552,10 @@
         <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2598,10 +2563,10 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2609,10 +2574,10 @@
         <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -2620,10 +2585,10 @@
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -2631,10 +2596,10 @@
         <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -2642,10 +2607,10 @@
         <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C17" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2653,10 +2618,10 @@
         <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -2664,105 +2629,94 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C21" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G21" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C22" t="s">
         <v>211</v>
       </c>
-      <c r="D22" t="s">
-        <v>212</v>
-      </c>
-      <c r="E22" t="s">
-        <v>213</v>
-      </c>
-      <c r="F22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G22" t="s">
-        <v>215</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C23" t="s">
-        <v>216</v>
+        <v>212</v>
+      </c>
+      <c r="D23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E23" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C24" t="s">
-        <v>217</v>
-      </c>
-      <c r="D24" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>300</v>
-      </c>
-      <c r="C26" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2791,59 +2745,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2854,10 +2808,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2872,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -2886,7 +2840,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2894,7 +2848,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2902,7 +2856,7 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2910,7 +2864,7 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -2918,7 +2872,7 @@
         <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2926,7 +2880,7 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2934,7 +2888,7 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2942,7 +2896,7 @@
         <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -2950,7 +2904,7 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -2958,7 +2912,7 @@
         <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2966,13 +2920,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -2980,23 +2934,23 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -3004,10 +2958,10 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -3015,15 +2969,15 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -3031,62 +2985,54 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
-        <v>242</v>
+        <v>238</v>
+      </c>
+      <c r="C21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>164</v>
+      <c r="A22" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="B22" t="s">
-        <v>243</v>
+        <v>275</v>
       </c>
       <c r="C22" t="s">
         <v>238</v>
       </c>
       <c r="D22" t="s">
-        <v>240</v>
+        <v>235</v>
+      </c>
+      <c r="E22" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
-        <v>279</v>
+      <c r="A23" s="9" t="s">
+        <v>277</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
-      </c>
-      <c r="C23" t="s">
-        <v>243</v>
-      </c>
-      <c r="D23" t="s">
-        <v>240</v>
-      </c>
-      <c r="E23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B24" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3115,25 +3061,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3141,138 +3087,138 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="D4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="D5" t="s">
-        <v>261</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C6" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D6" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3283,10 +3229,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3301,19 +3247,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3321,7 +3267,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3329,7 +3275,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3337,7 +3283,7 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3345,7 +3291,7 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3353,7 +3299,7 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3361,7 +3307,7 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3369,7 +3315,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3377,7 +3323,7 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3385,15 +3331,15 @@
         <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3401,23 +3347,23 @@
         <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3425,7 +3371,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3433,15 +3379,15 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -3449,47 +3395,47 @@
         <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -3497,43 +3443,43 @@
         <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>275</v>
+        <v>270</v>
+      </c>
+      <c r="C26" t="s">
+        <v>270</v>
+      </c>
+      <c r="D26" t="s">
+        <v>268</v>
+      </c>
+      <c r="E26" t="s">
+        <v>268</v>
+      </c>
+      <c r="F26" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>275</v>
-      </c>
-      <c r="C27" t="s">
-        <v>275</v>
-      </c>
-      <c r="D27" t="s">
-        <v>273</v>
-      </c>
-      <c r="E27" t="s">
-        <v>273</v>
-      </c>
-      <c r="F27" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -3541,101 +3487,93 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>149</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>275</v>
+        <v>268</v>
+      </c>
+      <c r="C29" t="s">
+        <v>268</v>
+      </c>
+      <c r="D29" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>273</v>
-      </c>
-      <c r="C30" t="s">
-        <v>273</v>
-      </c>
-      <c r="D30" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>27</v>
+      <c r="A32" s="9" t="s">
+        <v>277</v>
       </c>
       <c r="B32" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
-        <v>282</v>
+      <c r="A33" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="B36" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
-        <v>135</v>
+      <c r="A37" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B38" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update spectrum specification description in hydrodynamics DDS
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="302" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="368"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -349,9 +349,6 @@
     <t>Spreading Parameter for Wave Spectrum</t>
   </si>
   <si>
-    <t>Wave spectrum spreading factor for lease area.</t>
-  </si>
-  <si>
     <t>farm.spectrum_name</t>
   </si>
   <si>
@@ -697,9 +694,6 @@
     <t>Valid Value 5</t>
   </si>
   <si>
-    <t>Jonswap</t>
-  </si>
-  <si>
     <t>Pierson-Moskowitz</t>
   </si>
   <si>
@@ -917,6 +911,12 @@
   </si>
   <si>
     <t>filter.lease_area</t>
+  </si>
+  <si>
+    <t>JONSWAP</t>
+  </si>
+  <si>
+    <t>Wave spectrum spreading factor for lease area. Follows the COSINE 2s convention.</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1523,10 +1523,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>2</v>
@@ -1983,10 +1983,10 @@
         <v>102</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G25" s="24" t="s">
         <v>26</v>
@@ -2006,13 +2006,13 @@
         <v>105</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>106</v>
+        <v>295</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>26</v>
@@ -2023,22 +2023,22 @@
     </row>
     <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="25" t="s">
-        <v>109</v>
-      </c>
       <c r="E27" s="24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G27" s="24" t="s">
         <v>26</v>
@@ -2049,305 +2049,305 @@
     </row>
     <row r="28" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="C28" s="24" t="s">
+      <c r="D28" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="G28" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="C29" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="D29" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="H29" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="26" t="s">
+      <c r="D30" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="H30" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="D31" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="H31" s="26" t="s">
         <v>125</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="26" t="s">
+      <c r="D32" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="H32" s="26" t="s">
         <v>129</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="26" t="s">
         <v>131</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>132</v>
       </c>
       <c r="D33" s="27"/>
       <c r="H33" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="26" t="s">
+      <c r="D34" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="H34" s="26" t="s">
         <v>136</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="26" t="s">
+      <c r="D35" s="27" t="s">
         <v>139</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="D36" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="H36" s="26" t="s">
         <v>143</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="26" t="s">
         <v>145</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="D37" s="27"/>
       <c r="H37" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="C38" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="D38" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="H38" s="26" t="s">
         <v>151</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" s="26" t="s">
+      <c r="D39" s="27" t="s">
         <v>154</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="D40" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="H40" s="26" t="s">
         <v>158</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="C41" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="D41" s="25" t="s">
         <v>162</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>163</v>
       </c>
       <c r="G41" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="C42" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="D42" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="26" t="s">
         <v>170</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>171</v>
       </c>
       <c r="D44" s="27"/>
       <c r="H44" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="C45" s="26" t="s">
         <v>174</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>175</v>
       </c>
       <c r="D45" s="27"/>
       <c r="H45" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>176</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>177</v>
       </c>
       <c r="D46" s="25"/>
       <c r="G46" s="24" t="s">
@@ -2356,36 +2356,36 @@
     </row>
     <row r="47" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="B47" s="29" t="s">
-        <v>179</v>
-      </c>
       <c r="C47" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E47" s="29"/>
       <c r="F47" s="29"/>
       <c r="G47" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H47" s="29"/>
     </row>
     <row r="48" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" s="27" t="s">
         <v>277</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2419,22 +2419,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2442,10 +2442,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2453,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2464,10 +2464,10 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2475,10 +2475,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -2486,10 +2486,10 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -2497,10 +2497,10 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2508,10 +2508,10 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2519,10 +2519,10 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2530,10 +2530,10 @@
         <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2541,10 +2541,10 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2552,10 +2552,10 @@
         <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2563,10 +2563,10 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2574,10 +2574,10 @@
         <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -2585,10 +2585,10 @@
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -2596,10 +2596,10 @@
         <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -2607,10 +2607,10 @@
         <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2618,10 +2618,10 @@
         <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -2629,55 +2629,55 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" t="s">
         <v>206</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>207</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>208</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>209</v>
-      </c>
-      <c r="G21" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -2685,16 +2685,16 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C23" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" t="s">
         <v>212</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>213</v>
-      </c>
-      <c r="E23" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -2702,10 +2702,10 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -2713,10 +2713,10 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +2730,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2745,59 +2745,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" t="s">
         <v>222</v>
       </c>
-      <c r="D2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E2" t="s">
-        <v>224</v>
-      </c>
       <c r="F2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" t="s">
         <v>225</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>226</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>227</v>
-      </c>
-      <c r="E3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F3" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2826,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -2840,7 +2840,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2848,7 +2848,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2856,7 +2856,7 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2864,7 +2864,7 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -2872,7 +2872,7 @@
         <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2880,7 +2880,7 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2888,7 +2888,7 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2896,7 +2896,7 @@
         <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -2904,7 +2904,7 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -2912,7 +2912,7 @@
         <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2920,13 +2920,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -2934,23 +2934,23 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -2958,10 +2958,10 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2969,15 +2969,15 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2985,7 +2985,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2993,46 +2993,46 @@
         <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" t="s">
         <v>233</v>
-      </c>
-      <c r="D21" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3061,25 +3061,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3087,138 +3087,138 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" t="s">
         <v>246</v>
-      </c>
-      <c r="C2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" t="s">
         <v>249</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D5" t="s">
-        <v>256</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" t="s">
         <v>257</v>
-      </c>
-      <c r="C6" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" t="s">
         <v>257</v>
-      </c>
-      <c r="C7" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>276</v>
-      </c>
       <c r="C9" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>257</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3231,7 +3231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
@@ -3247,19 +3247,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3267,7 +3267,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3275,7 +3275,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3283,7 +3283,7 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3291,7 +3291,7 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3299,7 +3299,7 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3307,7 +3307,7 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3315,7 +3315,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3323,7 +3323,7 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3331,15 +3331,15 @@
         <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3347,23 +3347,23 @@
         <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3371,7 +3371,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3379,15 +3379,15 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -3395,23 +3395,23 @@
         <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -3419,15 +3419,15 @@
         <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -3435,7 +3435,7 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -3443,51 +3443,51 @@
         <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -3495,13 +3495,13 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -3509,7 +3509,7 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -3517,23 +3517,23 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -3541,7 +3541,7 @@
         <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -3549,31 +3549,31 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Numerous data model and test data fixes.
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="368"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="368" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -520,9 +520,6 @@
     <t>hydrodynamics: MetoceanConditions["Tp","Hs","Dir"].  NB: Wave only.</t>
   </si>
   <si>
-    <t>farm.mannings</t>
-  </si>
-  <si>
     <t>XGrid2D</t>
   </si>
   <si>
@@ -917,6 +914,9 @@
   </si>
   <si>
     <t>Wave time series data (Te, Hm0, Dir) keyed on date and time. Minimum of one year of hourly data for a representative point.</t>
+  </si>
+  <si>
+    <t>bathymetry.mannings</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1523,10 +1523,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>282</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>283</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>2</v>
@@ -1983,10 +1983,10 @@
         <v>102</v>
       </c>
       <c r="E25" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="F25" s="24" t="s">
         <v>286</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>287</v>
       </c>
       <c r="G25" s="24" t="s">
         <v>26</v>
@@ -2006,13 +2006,13 @@
         <v>105</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E26" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="F26" s="24" t="s">
         <v>286</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>287</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>26</v>
@@ -2035,10 +2035,10 @@
         <v>108</v>
       </c>
       <c r="E27" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="F27" s="24" t="s">
         <v>286</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>287</v>
       </c>
       <c r="G27" s="24" t="s">
         <v>26</v>
@@ -2052,7 +2052,7 @@
         <v>109</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>110</v>
@@ -2186,7 +2186,7 @@
         <v>140</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>141</v>
@@ -2272,7 +2272,7 @@
         <v>161</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G41" s="24" t="s">
         <v>26</v>
@@ -2283,71 +2283,71 @@
     </row>
     <row r="42" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B42" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="C42" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="D42" s="25" t="s">
         <v>165</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="D43" s="27" t="s">
         <v>269</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="26" t="s">
         <v>168</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>169</v>
       </c>
       <c r="D44" s="27"/>
       <c r="H44" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="C45" s="26" t="s">
         <v>172</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>173</v>
       </c>
       <c r="D45" s="27"/>
       <c r="H45" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>174</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>175</v>
       </c>
       <c r="D46" s="25"/>
       <c r="G46" s="24" t="s">
@@ -2356,36 +2356,36 @@
     </row>
     <row r="47" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="B47" s="29" t="s">
-        <v>177</v>
-      </c>
       <c r="C47" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E47" s="29"/>
       <c r="F47" s="29"/>
       <c r="G47" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H47" s="29"/>
     </row>
     <row r="48" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B48" s="26" t="s">
         <v>114</v>
       </c>
       <c r="C48" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="27" t="s">
         <v>275</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2419,22 +2419,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2442,10 +2442,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2453,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2464,10 +2464,10 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2475,10 +2475,10 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -2486,10 +2486,10 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -2497,10 +2497,10 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2508,10 +2508,10 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2519,10 +2519,10 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2530,10 +2530,10 @@
         <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2541,10 +2541,10 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2552,10 +2552,10 @@
         <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2563,10 +2563,10 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2574,10 +2574,10 @@
         <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -2585,10 +2585,10 @@
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -2596,10 +2596,10 @@
         <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -2607,10 +2607,10 @@
         <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2618,10 +2618,10 @@
         <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -2629,10 +2629,10 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -2640,10 +2640,10 @@
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -2651,22 +2651,22 @@
         <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" t="s">
         <v>204</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>205</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>206</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>207</v>
-      </c>
-      <c r="G21" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -2674,10 +2674,10 @@
         <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -2685,16 +2685,16 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" t="s">
         <v>210</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>211</v>
-      </c>
-      <c r="E23" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -2702,10 +2702,10 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -2713,10 +2713,10 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2745,19 +2745,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2765,19 +2765,19 @@
         <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" t="s">
         <v>220</v>
       </c>
-      <c r="E2" t="s">
-        <v>221</v>
-      </c>
       <c r="F2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -2785,19 +2785,19 @@
         <v>144</v>
       </c>
       <c r="B3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" t="s">
         <v>222</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>223</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>224</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>225</v>
-      </c>
-      <c r="F3" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2826,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -2840,7 +2840,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2848,7 +2848,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2856,7 +2856,7 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2864,7 +2864,7 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -2872,7 +2872,7 @@
         <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2880,7 +2880,7 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2888,7 +2888,7 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2896,7 +2896,7 @@
         <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -2904,7 +2904,7 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -2912,7 +2912,7 @@
         <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2920,13 +2920,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -2934,7 +2934,7 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -2942,7 +2942,7 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -2950,7 +2950,7 @@
         <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -2958,10 +2958,10 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2969,7 +2969,7 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2977,7 +2977,7 @@
         <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2985,7 +2985,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2993,7 +2993,7 @@
         <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -3001,38 +3001,38 @@
         <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" t="s">
         <v>271</v>
       </c>
-      <c r="B22" t="s">
-        <v>272</v>
-      </c>
       <c r="C22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3045,8 +3045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3061,25 +3061,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3087,90 +3087,90 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
         <v>243</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>244</v>
-      </c>
-      <c r="D2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" t="s">
         <v>246</v>
-      </c>
-      <c r="C3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" t="s">
         <v>246</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>247</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
         <v>246</v>
       </c>
-      <c r="C5" t="s">
-        <v>247</v>
-      </c>
       <c r="D5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
         <v>254</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>255</v>
-      </c>
-      <c r="D6" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -3178,47 +3178,47 @@
         <v>159</v>
       </c>
       <c r="B7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" t="s">
         <v>254</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>255</v>
-      </c>
-      <c r="D7" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>247</v>
-      </c>
       <c r="D8" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3247,19 +3247,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3267,7 +3267,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3275,7 +3275,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3283,7 +3283,7 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3291,7 +3291,7 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3299,7 +3299,7 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3307,7 +3307,7 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3315,7 +3315,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3323,7 +3323,7 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3331,7 +3331,7 @@
         <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3339,7 +3339,7 @@
         <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3347,7 +3347,7 @@
         <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -3355,7 +3355,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -3363,7 +3363,7 @@
         <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3371,7 +3371,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3379,7 +3379,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -3387,7 +3387,7 @@
         <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -3395,7 +3395,7 @@
         <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -3403,7 +3403,7 @@
         <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -3411,7 +3411,7 @@
         <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -3419,7 +3419,7 @@
         <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -3427,7 +3427,7 @@
         <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -3435,7 +3435,7 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -3443,7 +3443,7 @@
         <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -3451,7 +3451,7 @@
         <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -3459,19 +3459,19 @@
         <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -3479,7 +3479,7 @@
         <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -3487,7 +3487,7 @@
         <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -3495,13 +3495,13 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -3509,7 +3509,7 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -3517,15 +3517,15 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -3533,7 +3533,7 @@
         <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -3541,7 +3541,7 @@
         <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -3549,7 +3549,7 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -3557,7 +3557,7 @@
         <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -3565,7 +3565,7 @@
         <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -3573,7 +3573,7 @@
         <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove power law exponent from data model as only used with soulsby tidal profile formulation. Fix some DDS fields and reorder inputs to hydrodynamics module.
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="421" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="421" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <sheet name="Types" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$G$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ROOT!$A$1:$H$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Units!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="294">
   <si>
     <t>Identifier</t>
   </si>
@@ -298,18 +300,6 @@
     <t>hydrodynamics: Main_Direction.</t>
   </si>
   <si>
-    <t>farm.power_law_exponent</t>
-  </si>
-  <si>
-    <t>Tidal Velocity Shear Formula (Power Law) Exponent</t>
-  </si>
-  <si>
-    <t>Tidal: Exponent to be used in velocity shear formula.</t>
-  </si>
-  <si>
-    <t>hydrodynamics: VelocityShear. NB: Tidal only.</t>
-  </si>
-  <si>
     <t>Array Rated Power</t>
   </si>
   <si>
@@ -487,12 +477,6 @@
     <t>XGrid2D</t>
   </si>
   <si>
-    <t>Mannings Number</t>
-  </si>
-  <si>
-    <t>Mannings number at each point of the sea bottom</t>
-  </si>
-  <si>
     <t>XGrid3D</t>
   </si>
   <si>
@@ -583,9 +567,6 @@
     <t>blockage_ratio</t>
   </si>
   <si>
-    <t>power_law_exponent</t>
-  </si>
-  <si>
     <t>wave_spectrum_gamma</t>
   </si>
   <si>
@@ -721,12 +702,6 @@
     <t>Coefficient of Thrust</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -920,6 +895,27 @@
   </si>
   <si>
     <t>filter.device_tidal_power_performance</t>
+  </si>
+  <si>
+    <t>Units 4</t>
+  </si>
+  <si>
+    <t>s/m^{1/3}</t>
+  </si>
+  <si>
+    <t>Manning's Number</t>
+  </si>
+  <si>
+    <t>UTM x</t>
+  </si>
+  <si>
+    <t>UTM y</t>
+  </si>
+  <si>
+    <t>Time series of velocities, sea surface elevation and turbulence intensities for all lease area points. Two weeks of hourly data is typical.</t>
+  </si>
+  <si>
+    <t>Manning's number at each point of the sea bottom.</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1042,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1119,6 +1115,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -1493,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1526,10 +1528,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>2</v>
@@ -1539,859 +1541,879 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="A2" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>14</v>
-      </c>
+      <c r="A3" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>22</v>
+      <c r="A5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>31</v>
+      <c r="A7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>32</v>
+        <v>245</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="27"/>
+        <v>243</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="9" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="G11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="G12" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="G15" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>41</v>
+        <v>254</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>83</v>
+        <v>93</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>261</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>281</v>
+        <v>95</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>86</v>
+        <v>266</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>261</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>261</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>94</v>
+      <c r="A24" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>270</v>
+        <v>27</v>
       </c>
       <c r="G25" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>275</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="24" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="G27" s="24" t="s">
+      <c r="A27" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="26" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>8</v>
-      </c>
       <c r="H28" s="24" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>111</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
-        <v>285</v>
+        <v>119</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="H30" s="26" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
-        <v>286</v>
+        <v>123</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
-        <v>288</v>
+        <v>126</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
-        <v>289</v>
+        <v>32</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="D33" s="27"/>
-      <c r="H33" s="26" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="34" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>125</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D34" s="27"/>
       <c r="H34" s="26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
-        <v>127</v>
+        <v>274</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>129</v>
+        <v>106</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
-        <v>130</v>
+        <v>275</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>264</v>
+        <v>133</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
-        <v>134</v>
+        <v>271</v>
       </c>
       <c r="B37" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="D37" s="27"/>
-      <c r="H37" s="26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>276</v>
-      </c>
-      <c r="G41" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H41" s="24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>152</v>
+      <c r="D42" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H42" s="26" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>252</v>
+        <v>111</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
-        <v>154</v>
+        <v>278</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" s="27"/>
+        <v>139</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>140</v>
+      </c>
       <c r="H44" s="26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="27"/>
-      <c r="H45" s="26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="D46" s="25"/>
-      <c r="G46" s="24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45" s="24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>260</v>
-      </c>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="H47" s="29"/>
-    </row>
-    <row r="48" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>259</v>
+      <c r="H45" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="H47" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H47">
+    <sortState ref="A2:H48">
+      <sortCondition ref="A1:A48"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2399,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2422,22 +2444,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2445,10 +2467,10 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2456,10 +2478,10 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2467,10 +2489,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2478,10 +2500,10 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -2489,10 +2511,10 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -2500,10 +2522,10 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2511,10 +2533,10 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2522,10 +2544,10 @@
         <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2533,10 +2555,10 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2544,10 +2566,10 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2555,10 +2577,10 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2566,10 +2588,10 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C13" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2577,21 +2599,21 @@
         <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -2599,16 +2621,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -2616,21 +2638,21 @@
         <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -2638,70 +2660,59 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C21" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" t="s">
-        <v>272</v>
-      </c>
-      <c r="C23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D23" t="s">
-        <v>188</v>
-      </c>
-      <c r="E23" t="s">
-        <v>189</v>
-      </c>
-      <c r="F23" t="s">
-        <v>190</v>
-      </c>
-      <c r="G23" t="s">
-        <v>191</v>
+        <v>180</v>
+      </c>
+      <c r="D22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" t="s">
+        <v>183</v>
+      </c>
+      <c r="G22" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G23">
+  <autoFilter ref="A1:G22">
     <sortState ref="A2:G23">
       <sortCondition ref="B1:B23"/>
     </sortState>
@@ -2731,59 +2742,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2794,236 +2805,259 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.453125"/>
-    <col min="2" max="4" width="6.54296875"/>
-    <col min="5" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" customWidth="1"/>
+    <col min="6" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="B14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>284</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>280</v>
+        <v>211</v>
+      </c>
+      <c r="C15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B20" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="B21" t="s">
-        <v>218</v>
-      </c>
-      <c r="C21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>254</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="33" t="s">
+        <v>270</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
-      </c>
-      <c r="C22" t="s">
-        <v>218</v>
-      </c>
-      <c r="D22" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
-        <v>257</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E23">
+    <sortState ref="A2:E23">
+      <sortCondition ref="A1:A23"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3032,7 +3066,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3047,25 +3081,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3073,138 +3107,138 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
       <c r="D4" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
       <c r="D5" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D6" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>230</v>
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" t="s">
+        <v>291</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3215,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3233,19 +3267,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3253,7 +3287,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3261,7 +3295,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3269,7 +3303,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3277,7 +3311,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -3285,7 +3319,7 @@
         <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3293,7 +3327,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3301,7 +3335,7 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3309,7 +3343,7 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3317,15 +3351,15 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3333,23 +3367,23 @@
         <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B13" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3357,63 +3391,63 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B16" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>88</v>
+        <v>277</v>
       </c>
       <c r="B18" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="B20" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>288</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -3421,43 +3455,43 @@
         <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>250</v>
+        <v>241</v>
+      </c>
+      <c r="C25" t="s">
+        <v>241</v>
+      </c>
+      <c r="D25" t="s">
+        <v>239</v>
+      </c>
+      <c r="E25" t="s">
+        <v>239</v>
+      </c>
+      <c r="F25" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
-      </c>
-      <c r="C26" t="s">
-        <v>250</v>
-      </c>
-      <c r="D26" t="s">
-        <v>248</v>
-      </c>
-      <c r="E26" t="s">
-        <v>248</v>
-      </c>
-      <c r="F26" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -3465,101 +3499,93 @@
         <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>134</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>239</v>
+      </c>
+      <c r="C28" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
-      </c>
-      <c r="C29" t="s">
-        <v>248</v>
-      </c>
-      <c r="D29" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
-        <v>257</v>
+      <c r="A32" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>63</v>
+        <v>280</v>
       </c>
       <c r="B35" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
-        <v>289</v>
+      <c r="A36" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>127</v>
+        <v>281</v>
       </c>
       <c r="B37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B38" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched nogo area variables to PolygonDict structures
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="421" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="421" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
-    <sheet name="Tables" sheetId="2" r:id="rId2"/>
-    <sheet name="Valid Values" sheetId="3" r:id="rId3"/>
+    <sheet name="Labels" sheetId="5" r:id="rId2"/>
+    <sheet name="Types" sheetId="6" r:id="rId3"/>
     <sheet name="Units" sheetId="4" r:id="rId4"/>
-    <sheet name="Labels" sheetId="5" r:id="rId5"/>
-    <sheet name="Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Valid Values" sheetId="3" r:id="rId5"/>
+    <sheet name="Tables" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ROOT!$A$1:$H$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Tables!$A$1:$G$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Units!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="295">
   <si>
     <t>Identifier</t>
   </si>
@@ -144,9 +144,6 @@
     <t>farm.nogo_areas</t>
   </si>
   <si>
-    <t>PolygonListColumn</t>
-  </si>
-  <si>
     <t>Nogo Areas</t>
   </si>
   <si>
@@ -916,6 +913,12 @@
   </si>
   <si>
     <t>Manning's number at each point of the sea bottom.</t>
+  </si>
+  <si>
+    <t>PolygonDictColumn</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1528,10 +1531,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>256</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>257</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>2</v>
@@ -1542,36 +1545,36 @@
     </row>
     <row r="2" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>157</v>
-      </c>
       <c r="C2" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="G2" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
@@ -1580,22 +1583,22 @@
     </row>
     <row r="4" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>43</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
@@ -1622,36 +1625,36 @@
     </row>
     <row r="6" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="25" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>47</v>
       </c>
       <c r="G6" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="D7" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>51</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
@@ -1659,161 +1662,161 @@
         <v>8</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>243</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="D9" s="25" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>54</v>
       </c>
       <c r="G9" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="D10" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="G10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="24" t="s">
+      <c r="D11" s="25" t="s">
         <v>60</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>61</v>
       </c>
       <c r="G11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="24" t="s">
+      <c r="D12" s="25" t="s">
         <v>64</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>65</v>
       </c>
       <c r="G12" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="D13" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="D14" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>76</v>
       </c>
       <c r="G15" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1838,62 +1841,62 @@
     </row>
     <row r="17" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="D17" s="25" t="s">
         <v>101</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>102</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="24" t="s">
+      <c r="D18" s="25" t="s">
         <v>78</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="D19" s="25" t="s">
         <v>82</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>83</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1901,115 +1904,115 @@
         <v>35</v>
       </c>
       <c r="B20" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="D20" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>38</v>
       </c>
       <c r="G20" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="24" t="s">
+      <c r="D21" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>93</v>
-      </c>
       <c r="E21" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="F21" s="24" t="s">
         <v>260</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>261</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>96</v>
-      </c>
       <c r="D22" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E22" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="F22" s="24" t="s">
         <v>260</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>261</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="D23" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>99</v>
-      </c>
       <c r="E23" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="F23" s="24" t="s">
         <v>260</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>261</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="C24" s="26" t="s">
         <v>152</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>153</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
       <c r="H24" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -2034,16 +2037,16 @@
     </row>
     <row r="26" spans="1:8" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>155</v>
-      </c>
       <c r="D26" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>24</v>
@@ -2051,34 +2054,34 @@
     </row>
     <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="26" t="s">
         <v>148</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="26" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="C28" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>144</v>
-      </c>
       <c r="D28" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -2086,69 +2089,69 @@
         <v>24</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="26" t="s">
+      <c r="D29" s="27" t="s">
         <v>249</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="26" t="s">
+      <c r="D30" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="H30" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="D31" s="27" t="s">
         <v>124</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="C32" s="26" t="s">
+      <c r="D32" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="H32" s="26" t="s">
         <v>128</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -2165,56 +2168,56 @@
     </row>
     <row r="34" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="26" t="s">
         <v>130</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>131</v>
       </c>
       <c r="D34" s="27"/>
       <c r="H34" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B35" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="D35" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="H35" s="26" t="s">
         <v>106</v>
-      </c>
-      <c r="H35" s="26" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B36" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="D36" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="H36" s="26" t="s">
         <v>135</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>29</v>
@@ -2228,16 +2231,16 @@
     </row>
     <row r="38" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="25" t="s">
         <v>85</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>86</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -2245,12 +2248,12 @@
         <v>24</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>12</v>
@@ -2268,16 +2271,16 @@
     </row>
     <row r="40" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="27" t="s">
         <v>137</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>138</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
@@ -2286,7 +2289,7 @@
     </row>
     <row r="41" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>20</v>
@@ -2304,108 +2307,108 @@
     </row>
     <row r="42" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="H42" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="H42" s="26" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="27" t="s">
+      <c r="H43" s="26" t="s">
         <v>112</v>
-      </c>
-      <c r="H43" s="26" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="26" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C44" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="H44" s="26" t="s">
         <v>140</v>
-      </c>
-      <c r="H44" s="26" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="25" t="s">
         <v>88</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>89</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="27" t="s">
         <v>114</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>115</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
       <c r="G46" s="26"/>
       <c r="H46" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D47" s="27"/>
       <c r="H47" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2421,7 +2424,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.08984375"/>
+    <col min="2" max="8" width="20.36328125"/>
+    <col min="9" max="1025" width="8.54296875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
@@ -2429,311 +2629,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.54296875"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>282</v>
-      </c>
-      <c r="C6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>283</v>
-      </c>
-      <c r="C9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>283</v>
-      </c>
-      <c r="C10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>283</v>
-      </c>
-      <c r="C11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>282</v>
-      </c>
-      <c r="C13" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" t="s">
-        <v>283</v>
-      </c>
-      <c r="C14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" t="s">
-        <v>285</v>
-      </c>
-      <c r="C15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C16" t="s">
-        <v>186</v>
-      </c>
-      <c r="D16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" t="s">
-        <v>264</v>
-      </c>
-      <c r="C17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" t="s">
-        <v>264</v>
-      </c>
-      <c r="C18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>264</v>
-      </c>
-      <c r="C19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>264</v>
-      </c>
-      <c r="C20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>264</v>
-      </c>
-      <c r="C21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" t="s">
-        <v>263</v>
-      </c>
-      <c r="C22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22" t="s">
-        <v>182</v>
-      </c>
-      <c r="F22" t="s">
-        <v>183</v>
-      </c>
-      <c r="G22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:G22">
-    <sortState ref="A2:G23">
-      <sortCondition ref="B1:B23"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
     <col min="1" max="1" width="37.6328125"/>
-    <col min="2" max="6" width="20.36328125"/>
+    <col min="2" max="6" width="7.08984375"/>
     <col min="7" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
@@ -2742,64 +2639,330 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F2" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" t="s">
-        <v>202</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25" t="s">
+        <v>238</v>
+      </c>
+      <c r="F25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2824,16 +2987,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2841,96 +3004,96 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
         <v>245</v>
       </c>
-      <c r="B5" t="s">
-        <v>246</v>
-      </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2938,116 +3101,116 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3063,213 +3226,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.08984375"/>
-    <col min="2" max="8" width="20.36328125"/>
-    <col min="9" max="1025" width="8.54296875"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C5" t="s">
-        <v>291</v>
-      </c>
-      <c r="D5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C8" t="s">
-        <v>291</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="B10" t="s">
-        <v>290</v>
-      </c>
-      <c r="C10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.6328125"/>
-    <col min="2" max="6" width="7.08984375"/>
+    <col min="2" max="6" width="20.36328125"/>
     <col min="7" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
@@ -3278,329 +3244,369 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B13" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B16" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B18" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B19" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" t="s">
-        <v>241</v>
-      </c>
-      <c r="C25" t="s">
-        <v>241</v>
-      </c>
-      <c r="D25" t="s">
-        <v>239</v>
-      </c>
-      <c r="E25" t="s">
-        <v>239</v>
-      </c>
-      <c r="F25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>239</v>
-      </c>
-      <c r="C28" t="s">
-        <v>239</v>
-      </c>
-      <c r="D28" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="B31" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="B35" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B37" t="s">
-        <v>239</v>
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.54296875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>263</v>
+      </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G22">
+    <sortState ref="A2:G23">
+      <sortCondition ref="B1:B23"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add single wave device power matrix as output from hydrodynamics module
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,8 +20,11 @@
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Tables!$A$1:$G$22</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Units!$A$1:$E$23</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ROOT!$A$1:$H$47</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Units!$A$1:$E$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Units!$A$1:$E$23</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Tables!$A$1:$G$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tables!$A$1:$G$22</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="298">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -608,6 +611,15 @@
     <t xml:space="preserve">Treat as user option</t>
   </si>
   <si>
+    <t xml:space="preserve">device.wave_power_matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Device Power Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power matrix for the isolated wave energy device.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Label 1</t>
   </si>
   <si>
@@ -747,6 +759,9 @@
   </si>
   <si>
     <t xml:space="preserve">s/m^{1/3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kW</t>
   </si>
   <si>
     <t xml:space="preserve">Valid Value 1</t>
@@ -924,7 +939,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -954,12 +969,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1011,7 +1020,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1035,15 +1044,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1064,15 +1069,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1084,14 +1089,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1100,23 +1097,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1132,6 +1125,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1140,23 +1141,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1172,12 +1161,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
@@ -1185,7 +1170,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 40% - Accent1" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1267,10 +1251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:BA48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="1" sqref="A11:D11 B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1280,7 +1264,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="99.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="107.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="0" width="8.54"/>
@@ -1333,55 +1317,55 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+    <row r="5" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="8"/>
@@ -1393,793 +1377,855 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+    <row r="8" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" s="10" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="6" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" s="10" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="6" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
+    <row r="24" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" s="10" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="6" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
+    <row r="27" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16" t="s">
+      <c r="D27" s="15"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" s="16" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="13" customFormat="true" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
+    <row r="29" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
+    <row r="30" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="31" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
+    <row r="31" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
+    <row r="32" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="s">
+    <row r="33" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D33" s="18"/>
-    </row>
-    <row r="34" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="H34" s="16" t="s">
+      <c r="D34" s="15"/>
+      <c r="H34" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="35" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="s">
+    <row r="35" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="36" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="s">
+    <row r="36" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="37" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="s">
+    <row r="37" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="15" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10" t="s">
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="39" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19" t="s">
+    <row r="39" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17" t="s">
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-    </row>
-    <row r="41" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19" t="s">
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="42" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="17" t="s">
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="13" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="43" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="17" t="s">
+    <row r="43" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H43" s="13" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="44" s="16" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="17" t="s">
+    <row r="44" s="13" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H44" s="13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="45" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="H45" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" s="21" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="s">
+    <row r="46" s="18" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16" t="s">
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="47" s="16" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="17" t="s">
+    <row r="47" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D47" s="18"/>
-      <c r="H47" s="16" t="s">
+      <c r="D47" s="15"/>
+      <c r="H47" s="13" t="s">
         <v>190</v>
       </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="20"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="20"/>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
+      <c r="Z48" s="20"/>
+      <c r="AA48" s="20"/>
+      <c r="AB48" s="20"/>
+      <c r="AC48" s="20"/>
+      <c r="AD48" s="20"/>
+      <c r="AE48" s="20"/>
+      <c r="AF48" s="20"/>
+      <c r="AG48" s="20"/>
+      <c r="AH48" s="20"/>
+      <c r="AI48" s="20"/>
+      <c r="AJ48" s="20"/>
+      <c r="AK48" s="20"/>
+      <c r="AL48" s="20"/>
+      <c r="AM48" s="20"/>
+      <c r="AN48" s="20"/>
+      <c r="AO48" s="20"/>
+      <c r="AP48" s="20"/>
+      <c r="AQ48" s="20"/>
+      <c r="AR48" s="20"/>
+      <c r="AS48" s="20"/>
+      <c r="AT48" s="20"/>
+      <c r="AU48" s="20"/>
+      <c r="AV48" s="20"/>
+      <c r="AW48" s="20"/>
+      <c r="AX48" s="20"/>
+      <c r="AY48" s="20"/>
+      <c r="AZ48" s="20"/>
+      <c r="BA48" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H47"/>
@@ -2199,10 +2245,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2213,179 +2259,193 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="25" t="s">
+      <c r="B11" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="C11" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="D11" s="0" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2407,7 +2467,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A11:D11 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2418,329 +2478,329 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>220</v>
       </c>
+      <c r="D1" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>144</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>168</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>172</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>176</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>180</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>184</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>93</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>96</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>113</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>129</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>103</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="25" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="26" t="s">
         <v>122</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="26" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="26" t="s">
         <v>188</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="16" t="s">
         <v>126</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="16" t="s">
         <v>161</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2759,10 +2819,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="A11:D11 A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2774,234 +2834,268 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>228</v>
       </c>
+      <c r="C1" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D5" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>229</v>
-      </c>
       <c r="D15" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="23" t="s">
         <v>118</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" s="0" t="s">
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="E25" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>237</v>
+      <c r="C26" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3025,7 +3119,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A11:D11 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3036,63 +3130,63 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="F1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>242</v>
       </c>
+      <c r="C1" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>96</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3114,7 +3208,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A11:D11 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3130,278 +3224,278 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>258</v>
       </c>
+      <c r="D1" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="C12" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>267</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>77</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>93</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>96</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>282</v>
-      </c>
       <c r="C21" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing mannings number as an input and all database processing associated to it.
Reword device spacing variables.
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE62FF5-F2C1-4BFF-9554-6381C8536AAA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{428CB2C0-24C9-4F54-A91E-C8DD3570D297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,15 @@
     <sheet name="Tables" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">ROOT!$A$1:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">ROOT!$A$1:$H$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">Tables!$A$1:$G$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">Units!$A$1:$E$23</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="0">ROOT!$A$1:$H$46</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">ROOT!$A$1:$H$45</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">Tables!$A$1:$G$22</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="3">Units!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="286">
   <si>
     <t>Identifier</t>
   </si>
@@ -64,18 +65,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>bathymetry.mannings</t>
-  </si>
-  <si>
-    <t>XGrid2D</t>
-  </si>
-  <si>
-    <t>Manning's Number</t>
-  </si>
-  <si>
-    <t>Manning's number at each point of the sea bottom.</t>
-  </si>
-  <si>
     <t>device.bidirection</t>
   </si>
   <si>
@@ -721,9 +710,6 @@
     <t>MWh</t>
   </si>
   <si>
-    <t>s/m^{1/3}</t>
-  </si>
-  <si>
     <t>kW</t>
   </si>
   <si>
@@ -895,29 +881,29 @@
     <t>direction</t>
   </si>
   <si>
-    <t>Minimum distance between devices in x direction</t>
-  </si>
-  <si>
-    <t>Minimum allowed spacing between device in the array in x direction.</t>
-  </si>
-  <si>
-    <t>Minimum distance between devices in y direction</t>
-  </si>
-  <si>
-    <t>Minimum allowed spacing between device in the array in y direction.</t>
-  </si>
-  <si>
     <t>Distance between the turbine and the axis of the device in case of MCT device (two hubs). In the case of just one hub this value is set to zero.</t>
   </si>
   <si>
     <t>The number of "slices" from the tidal energy time series to be used to evaluate the energy generated.</t>
+  </si>
+  <si>
+    <t>Minimum distance between devices in the transverse direction (perpendicular to the array orientation). Also known as the column spacing.</t>
+  </si>
+  <si>
+    <t>Minimum Transverse Device Spacing</t>
+  </si>
+  <si>
+    <t>Minimum Longitudinal Device Spacing</t>
+  </si>
+  <si>
+    <t>Minimum distance between devices in the longitudinal direction (parallel to the array orientation). Also known as the row spacing.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -939,6 +925,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1008,7 +1001,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1061,13 +1054,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1453,21 +1440,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA47"/>
+  <dimension ref="A1:BA46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="99.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="107.28515625" customWidth="1"/>
     <col min="9" max="1020" width="8.5703125" customWidth="1"/>
     <col min="1021" max="1025" width="8.7109375" customWidth="1"/>
@@ -1499,7 +1486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1512,59 +1499,61 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>23</v>
@@ -1572,46 +1561,46 @@
       <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1620,7 +1609,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>34</v>
@@ -1629,70 +1618,70 @@
         <v>35</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="B10" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>286</v>
-      </c>
       <c r="G10" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1700,7 +1689,7 @@
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>44</v>
@@ -1709,78 +1698,78 @@
         <v>45</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>289</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>60</v>
@@ -1789,18 +1778,18 @@
         <v>61</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>64</v>
@@ -1809,38 +1798,38 @@
         <v>65</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>74</v>
@@ -1848,115 +1837,115 @@
       <c r="D19" s="6" t="s">
         <v>75</v>
       </c>
+      <c r="E19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="G19" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="G20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="14"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12" t="s">
+      <c r="D23" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>95</v>
@@ -1965,66 +1954,60 @@
         <v>96</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="14"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="C26" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="D26" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="5" t="s">
+    </row>
+    <row r="27" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="C27" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="5" t="s">
+      <c r="D27" s="14" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2033,12 +2016,15 @@
         <v>108</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="D28" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="H28" s="12" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2047,7 +2033,7 @@
         <v>112</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>113</v>
@@ -2055,16 +2041,13 @@
       <c r="D29" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="30" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>117</v>
@@ -2072,47 +2055,50 @@
       <c r="D30" s="14" t="s">
         <v>118</v>
       </c>
+      <c r="H30" s="12" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="31" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>123</v>
-      </c>
+      <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="D32" s="14"/>
+      <c r="H32" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="12" t="s">
+      <c r="D33" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="14"/>
       <c r="H33" s="12" t="s">
         <v>129</v>
       </c>
@@ -2122,131 +2108,131 @@
         <v>130</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H35" s="12" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="D36" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="C37" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H37" s="5" t="s">
+      <c r="D37" s="16" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="38" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="D38" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="B39" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="D40" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="H40" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>158</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>159</v>
@@ -2258,12 +2244,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" s="12" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>162</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>163</v>
@@ -2275,160 +2261,143 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:53" s="12" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" s="12" t="s">
+      <c r="B43" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="G43" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H43" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:53" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="G44" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H44" s="5" t="s">
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:53" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>174</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>175</v>
       </c>
       <c r="D45" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="H45" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12" t="s">
+    </row>
+    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="46" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="B46" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="12" t="s">
+      <c r="D46" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
-      <c r="S47" s="19"/>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19"/>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="19"/>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="19"/>
-      <c r="AD47" s="19"/>
-      <c r="AE47" s="19"/>
-      <c r="AF47" s="19"/>
-      <c r="AG47" s="19"/>
-      <c r="AH47" s="19"/>
-      <c r="AI47" s="19"/>
-      <c r="AJ47" s="19"/>
-      <c r="AK47" s="19"/>
-      <c r="AL47" s="19"/>
-      <c r="AM47" s="19"/>
-      <c r="AN47" s="19"/>
-      <c r="AO47" s="19"/>
-      <c r="AP47" s="19"/>
-      <c r="AQ47" s="19"/>
-      <c r="AR47" s="19"/>
-      <c r="AS47" s="19"/>
-      <c r="AT47" s="19"/>
-      <c r="AU47" s="19"/>
-      <c r="AV47" s="19"/>
-      <c r="AW47" s="19"/>
-      <c r="AX47" s="19"/>
-      <c r="AY47" s="19"/>
-      <c r="AZ47" s="19"/>
-      <c r="BA47" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="19"/>
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="19"/>
+      <c r="AC46" s="19"/>
+      <c r="AD46" s="19"/>
+      <c r="AE46" s="19"/>
+      <c r="AF46" s="19"/>
+      <c r="AG46" s="19"/>
+      <c r="AH46" s="19"/>
+      <c r="AI46" s="19"/>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
+      <c r="AL46" s="19"/>
+      <c r="AM46" s="19"/>
+      <c r="AN46" s="19"/>
+      <c r="AO46" s="19"/>
+      <c r="AP46" s="19"/>
+      <c r="AQ46" s="19"/>
+      <c r="AR46" s="19"/>
+      <c r="AS46" s="19"/>
+      <c r="AT46" s="19"/>
+      <c r="AU46" s="19"/>
+      <c r="AV46" s="19"/>
+      <c r="AW46" s="19"/>
+      <c r="AX46" s="19"/>
+      <c r="AY46" s="19"/>
+      <c r="AZ46" s="19"/>
+      <c r="BA46" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
@@ -2438,169 +2407,158 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="C2" t="s">
         <v>188</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="D2" t="s">
         <v>189</v>
       </c>
-      <c r="H1" s="20" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>191</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>192</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" s="21" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F3" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" s="21" t="s">
         <v>195</v>
       </c>
+      <c r="H3" s="21" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>89</v>
+      <c r="A4" s="24" t="s">
+        <v>94</v>
       </c>
       <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" s="21" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
         <v>198</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="C5" t="s">
         <v>199</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="D5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="C7" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="H5" s="21" t="s">
+      <c r="D7" s="21" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>204</v>
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" t="s">
-        <v>204</v>
+        <v>199</v>
+      </c>
+      <c r="D9" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2614,7 +2572,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" activeCellId="1" sqref="A1:F37"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2629,325 +2587,325 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="20" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="20" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="20" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="B17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="B18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="B20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>174</v>
-      </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>77</v>
+      <c r="A22" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>83</v>
+      <c r="A23" s="24" t="s">
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>86</v>
+      <c r="A24" s="24" t="s">
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>103</v>
+      <c r="A25" s="24" t="s">
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>119</v>
+      <c r="A26" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>127</v>
+      <c r="A27" s="24" t="s">
+        <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>53</v>
+      <c r="A28" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>72</v>
+      <c r="A29" s="24" t="s">
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>93</v>
+      <c r="A30" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B32" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>116</v>
-      </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>151</v>
+      <c r="A37" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2958,10 +2916,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" activeCellId="1" sqref="A1:E26"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,268 +2935,253 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="20" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>216</v>
       </c>
-      <c r="D1" s="20" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="C5" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D5" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>221</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" t="s">
         <v>222</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E24" t="s">
         <v>223</v>
       </c>
-      <c r="E5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" t="s">
-        <v>222</v>
-      </c>
-      <c r="C15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" t="s">
-        <v>219</v>
-      </c>
-      <c r="C19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B20" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" t="s">
-        <v>219</v>
-      </c>
-      <c r="C24" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="B25" t="s">
-        <v>222</v>
-      </c>
-      <c r="C25" t="s">
-        <v>219</v>
-      </c>
-      <c r="D25" t="s">
-        <v>223</v>
-      </c>
       <c r="E25" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" t="s">
-        <v>222</v>
-      </c>
-      <c r="C26" t="s">
-        <v>219</v>
-      </c>
-      <c r="D26" t="s">
-        <v>223</v>
-      </c>
-      <c r="E26" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E23" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -3249,13 +3192,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" activeCellId="1" sqref="A1:F3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" customWidth="1"/>
-    <col min="2" max="6" width="20.42578125" customWidth="1"/>
+    <col min="2" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3264,59 +3207,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C2" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D2" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E2" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
         <v>234</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>235</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>236</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>237</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F3" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3330,18 +3273,13 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" activeCellId="1" sqref="A1:G22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="35.7109375" customWidth="1"/>
     <col min="8" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3350,278 +3288,277 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
         <v>245</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="C2" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D2" t="s">
         <v>247</v>
       </c>
-      <c r="F1" s="20" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>248</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="C3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" t="s">
         <v>250</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" t="s">
         <v>251</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>253</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>253</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>253</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>253</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C11" t="s">
         <v>258</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C14" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>253</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="D16" t="s">
+        <v>266</v>
+      </c>
+      <c r="E16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>267</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B17" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>269</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C18" t="s">
         <v>270</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" t="s">
         <v>271</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>268</v>
+      </c>
+      <c r="C20" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C21" t="s">
         <v>273</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" t="s">
-        <v>273</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C22" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>273</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D22" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" t="s">
-        <v>273</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E22" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" t="s">
-        <v>273</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="F22" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="G22" t="s">
         <v>279</v>
       </c>
-      <c r="C22" t="s">
-        <v>280</v>
-      </c>
-      <c r="D22" t="s">
-        <v>281</v>
-      </c>
-      <c r="E22" t="s">
-        <v>282</v>
-      </c>
-      <c r="F22" t="s">
-        <v>283</v>
-      </c>
-      <c r="G22" t="s">
-        <v>284</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G22" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Add options.tidal_use_all_steps variable to calculate tidal hydrodynamics using all time steps
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{428CB2C0-24C9-4F54-A91E-C8DD3570D297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C21450-2BFD-412C-AB98-572285439B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <definedName name="_FilterDatabase_0" localSheetId="3">Units!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="289">
   <si>
     <t>Identifier</t>
   </si>
@@ -897,6 +896,15 @@
   </si>
   <si>
     <t>Minimum distance between devices in the longitudinal direction (parallel to the array orientation). Also known as the row spacing.</t>
+  </si>
+  <si>
+    <t>options.tidal_use_all_steps</t>
+  </si>
+  <si>
+    <t>Use all Tidal Timesteps</t>
+  </si>
+  <si>
+    <t>Use all tidal time series steps for energy calculation. This ignores the tidal probability bins setting and may add significant computational time. Defaults to False.</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1041,11 +1049,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1056,6 +1059,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1440,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1461,7 @@
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="107.28515625" customWidth="1"/>
+    <col min="8" max="8" width="114.28515625" customWidth="1"/>
     <col min="9" max="1020" width="8.5703125" customWidth="1"/>
     <col min="1021" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
@@ -1486,7 +1492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1499,6 +1505,8 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
@@ -1528,7 +1536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -1541,6 +1549,8 @@
       <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1548,7 +1558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1570,7 +1580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
@@ -1583,8 +1593,12 @@
       <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -1597,6 +1611,8 @@
       <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1604,7 +1620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -1617,6 +1633,8 @@
       <c r="D8" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
@@ -1637,6 +1655,8 @@
       <c r="D9" s="6" t="s">
         <v>282</v>
       </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1644,7 +1664,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
@@ -1657,6 +1677,8 @@
       <c r="D10" s="6" t="s">
         <v>285</v>
       </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1664,7 +1686,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -1677,6 +1699,8 @@
       <c r="D11" s="6" t="s">
         <v>41</v>
       </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1684,7 +1708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
@@ -1697,6 +1721,8 @@
       <c r="D12" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1704,7 +1730,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>47</v>
       </c>
@@ -1717,6 +1743,8 @@
       <c r="D13" s="6" t="s">
         <v>280</v>
       </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1724,7 +1752,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>49</v>
       </c>
@@ -1737,6 +1765,8 @@
       <c r="D14" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1744,7 +1774,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>54</v>
       </c>
@@ -1757,6 +1787,8 @@
       <c r="D15" s="6" t="s">
         <v>57</v>
       </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
@@ -1764,7 +1796,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>59</v>
       </c>
@@ -1777,6 +1809,8 @@
       <c r="D16" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1784,7 +1818,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>63</v>
       </c>
@@ -1797,6 +1831,8 @@
       <c r="D17" s="6" t="s">
         <v>65</v>
       </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
         <v>66</v>
       </c>
@@ -1804,7 +1840,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>68</v>
       </c>
@@ -1817,6 +1853,8 @@
       <c r="D18" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
         <v>66</v>
       </c>
@@ -1824,7 +1862,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>73</v>
       </c>
@@ -1850,7 +1888,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>79</v>
       </c>
@@ -1876,7 +1914,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>82</v>
       </c>
@@ -1902,7 +1940,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>85</v>
       </c>
@@ -1920,7 +1958,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>89</v>
       </c>
@@ -1933,6 +1971,8 @@
       <c r="D23" s="6" t="s">
         <v>92</v>
       </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="5" t="s">
         <v>66</v>
       </c>
@@ -1940,7 +1980,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>94</v>
       </c>
@@ -1953,11 +1993,14 @@
       <c r="D24" s="6" t="s">
         <v>96</v>
       </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>97</v>
       </c>
@@ -1975,7 +2018,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>99</v>
       </c>
@@ -1997,7 +2040,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>104</v>
       </c>
@@ -2010,8 +2053,12 @@
       <c r="D27" s="14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>108</v>
       </c>
@@ -2024,11 +2071,14 @@
       <c r="D28" s="14" t="s">
         <v>110</v>
       </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>112</v>
       </c>
@@ -2041,8 +2091,12 @@
       <c r="D29" s="14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>115</v>
       </c>
@@ -2055,11 +2109,14 @@
       <c r="D30" s="14" t="s">
         <v>118</v>
       </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>120</v>
       </c>
@@ -2070,8 +2127,12 @@
         <v>122</v>
       </c>
       <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>123</v>
       </c>
@@ -2082,11 +2143,14 @@
         <v>124</v>
       </c>
       <c r="D32" s="14"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>126</v>
       </c>
@@ -2099,11 +2163,14 @@
       <c r="D33" s="14" t="s">
         <v>128</v>
       </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>130</v>
       </c>
@@ -2116,11 +2183,14 @@
       <c r="D34" s="14" t="s">
         <v>133</v>
       </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>135</v>
       </c>
@@ -2133,8 +2203,12 @@
       <c r="D35" s="14" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="36" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>139</v>
       </c>
@@ -2156,7 +2230,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>143</v>
       </c>
@@ -2174,7 +2248,7 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>147</v>
       </c>
@@ -2192,7 +2266,7 @@
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
     </row>
-    <row r="39" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>150</v>
       </c>
@@ -2210,7 +2284,7 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>154</v>
       </c>
@@ -2223,11 +2297,14 @@
       <c r="D40" s="14" t="s">
         <v>156</v>
       </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>158</v>
       </c>
@@ -2240,11 +2317,14 @@
       <c r="D41" s="14" t="s">
         <v>160</v>
       </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="12" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>162</v>
       </c>
@@ -2257,11 +2337,14 @@
       <c r="D42" s="14" t="s">
         <v>164</v>
       </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>166</v>
       </c>
@@ -2274,6 +2357,8 @@
       <c r="D43" s="6" t="s">
         <v>168</v>
       </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="5" t="s">
         <v>66</v>
       </c>
@@ -2281,7 +2366,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:53" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>170</v>
       </c>
@@ -2301,7 +2386,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>174</v>
       </c>
@@ -2314,71 +2399,48 @@
       <c r="D45" s="14" t="s">
         <v>281</v>
       </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
       <c r="H45" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="19"/>
-      <c r="AD46" s="19"/>
-      <c r="AE46" s="19"/>
-      <c r="AF46" s="19"/>
-      <c r="AG46" s="19"/>
-      <c r="AH46" s="19"/>
-      <c r="AI46" s="19"/>
-      <c r="AJ46" s="19"/>
-      <c r="AK46" s="19"/>
-      <c r="AL46" s="19"/>
-      <c r="AM46" s="19"/>
-      <c r="AN46" s="19"/>
-      <c r="AO46" s="19"/>
-      <c r="AP46" s="19"/>
-      <c r="AQ46" s="19"/>
-      <c r="AR46" s="19"/>
-      <c r="AS46" s="19"/>
-      <c r="AT46" s="19"/>
-      <c r="AU46" s="19"/>
-      <c r="AV46" s="19"/>
-      <c r="AW46" s="19"/>
-      <c r="AX46" s="19"/>
-      <c r="AY46" s="19"/>
-      <c r="AZ46" s="19"/>
-      <c r="BA46" s="19"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -2403,33 +2465,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B2" t="s">
@@ -2443,7 +2505,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>85</v>
       </c>
       <c r="B3" t="s">
@@ -2455,21 +2517,21 @@
       <c r="D3" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="18" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B4" t="s">
@@ -2481,21 +2543,21 @@
       <c r="D4" t="s">
         <v>197</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="18" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B5" t="s">
@@ -2509,7 +2571,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B6" t="s">
@@ -2523,21 +2585,21 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>135</v>
       </c>
       <c r="B8" t="s">
@@ -2548,7 +2610,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>177</v>
       </c>
       <c r="B9" t="s">
@@ -2569,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2583,27 +2645,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -2611,7 +2673,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
@@ -2619,7 +2681,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
@@ -2627,7 +2689,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
@@ -2635,7 +2697,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
@@ -2643,7 +2705,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
@@ -2651,7 +2713,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B8" t="s">
@@ -2659,7 +2721,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B9" t="s">
@@ -2667,7 +2729,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B10" t="s">
@@ -2675,7 +2737,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
@@ -2683,7 +2745,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B12" t="s">
@@ -2691,7 +2753,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B13" t="s">
@@ -2699,7 +2761,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B14" t="s">
@@ -2707,7 +2769,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B15" t="s">
@@ -2715,7 +2777,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B16" t="s">
@@ -2723,7 +2785,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>154</v>
       </c>
       <c r="B17" t="s">
@@ -2731,7 +2793,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B18" t="s">
@@ -2739,7 +2801,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="21" t="s">
         <v>162</v>
       </c>
       <c r="B19" t="s">
@@ -2747,7 +2809,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="21" t="s">
         <v>166</v>
       </c>
       <c r="B20" t="s">
@@ -2755,7 +2817,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="21" t="s">
         <v>170</v>
       </c>
       <c r="B21" t="s">
@@ -2763,7 +2825,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="21" t="s">
         <v>73</v>
       </c>
       <c r="B22" t="s">
@@ -2771,7 +2833,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="21" t="s">
         <v>79</v>
       </c>
       <c r="B23" t="s">
@@ -2779,7 +2841,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B24" t="s">
@@ -2787,7 +2849,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B25" t="s">
@@ -2807,7 +2869,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="21" t="s">
         <v>115</v>
       </c>
       <c r="B26" t="s">
@@ -2815,7 +2877,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="21" t="s">
         <v>123</v>
       </c>
       <c r="B27" t="s">
@@ -2823,7 +2885,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B28" t="s">
@@ -2837,7 +2899,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B29" t="s">
@@ -2845,7 +2907,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B30" t="s">
@@ -2853,7 +2915,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="21" t="s">
         <v>104</v>
       </c>
       <c r="B31" t="s">
@@ -2861,7 +2923,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B32" t="s">
@@ -2869,7 +2931,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
@@ -2877,7 +2939,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B34" t="s">
@@ -2885,7 +2947,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="21" t="s">
         <v>174</v>
       </c>
       <c r="B35" t="s">
@@ -2893,7 +2955,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="21" t="s">
         <v>112</v>
       </c>
       <c r="B36" t="s">
@@ -2901,11 +2963,19 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="21" t="s">
         <v>147</v>
       </c>
       <c r="B37" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="B38" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2931,24 +3001,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -2956,7 +3026,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
@@ -2964,7 +3034,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
@@ -2972,7 +3042,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
@@ -2989,7 +3059,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
@@ -2997,7 +3067,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
@@ -3005,7 +3075,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
@@ -3013,7 +3083,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B9" t="s">
@@ -3021,7 +3091,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B10" t="s">
@@ -3029,7 +3099,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B11" t="s">
@@ -3037,7 +3107,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B12" t="s">
@@ -3045,7 +3115,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B13" t="s">
@@ -3059,7 +3129,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B14" t="s">
@@ -3067,7 +3137,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B15" t="s">
@@ -3081,7 +3151,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="21" t="s">
         <v>104</v>
       </c>
       <c r="B16" t="s">
@@ -3089,7 +3159,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B17" t="s">
@@ -3097,7 +3167,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B18" t="s">
@@ -3105,7 +3175,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="21" t="s">
         <v>135</v>
       </c>
       <c r="B19" t="s">
@@ -3116,7 +3186,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B20" t="s">
@@ -3124,7 +3194,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="21" t="s">
         <v>147</v>
       </c>
       <c r="B21" t="s">
@@ -3132,7 +3202,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="21" t="s">
         <v>150</v>
       </c>
       <c r="B22" t="s">
@@ -3140,7 +3210,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="21" t="s">
         <v>166</v>
       </c>
       <c r="B23" t="s">
@@ -3148,7 +3218,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="21" t="s">
         <v>177</v>
       </c>
       <c r="B24" t="s">
@@ -3165,7 +3235,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B25" t="s">
@@ -3203,27 +3273,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B2" t="s">
@@ -3243,7 +3313,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>123</v>
       </c>
       <c r="B3" t="s">
@@ -3284,30 +3354,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B2" t="s">
@@ -3321,7 +3391,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -3332,7 +3402,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
@@ -3343,7 +3413,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
@@ -3354,7 +3424,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
@@ -3365,7 +3435,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
@@ -3376,7 +3446,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
@@ -3387,7 +3457,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B9" t="s">
@@ -3398,7 +3468,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B10" t="s">
@@ -3409,7 +3479,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B11" t="s">
@@ -3420,7 +3490,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" t="s">
@@ -3431,7 +3501,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B13" t="s">
@@ -3442,7 +3512,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B14" t="s">
@@ -3453,7 +3523,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
@@ -3464,7 +3534,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B16" t="s">
@@ -3481,7 +3551,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B17" t="s">
@@ -3492,7 +3562,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>73</v>
       </c>
       <c r="B18" t="s">
@@ -3503,7 +3573,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="21" t="s">
         <v>79</v>
       </c>
       <c r="B19" t="s">
@@ -3514,7 +3584,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B20" t="s">
@@ -3525,7 +3595,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B21" t="s">
@@ -3536,7 +3606,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B22" t="s">

</xml_diff>

<commit_message>
Implement maximum and minimum limits on SimpleData structures
Fixes https://github.com/DTOcean/dtocean/issues/10
</commit_message>
<xml_diff>
--- a/dds/hydrodynamics.xlsx
+++ b/dds/hydrodynamics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC2DDC-E289-466A-9C61-7D4C9754E9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420BF1C8-189A-4CB2-AD03-E3237838A4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,17 @@
     <sheet name="Types" sheetId="3" r:id="rId3"/>
     <sheet name="Units" sheetId="4" r:id="rId4"/>
     <sheet name="Valid Values" sheetId="5" r:id="rId5"/>
-    <sheet name="Tables" sheetId="6" r:id="rId6"/>
+    <sheet name="Minimum Equals" sheetId="7" r:id="rId6"/>
+    <sheet name="Minimums" sheetId="9" r:id="rId7"/>
+    <sheet name="Maximum Equals" sheetId="10" r:id="rId8"/>
+    <sheet name="Tables" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">ROOT!$A$1:$H$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5">Tables!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ROOT!$A$1:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8">Tables!$A$1:$G$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">Units!$A$1:$E$23</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">ROOT!$A$1:$H$45</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">Tables!$A$1:$G$22</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="8">Tables!$A$1:$G$22</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="3">Units!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="287">
   <si>
     <t>Identifier</t>
   </si>
@@ -1452,10 +1455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -1758,7 +1762,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1780,7 +1784,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>68</v>
       </c>
@@ -1946,7 +1950,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="17" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>85</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>88</v>
       </c>
@@ -1982,7 +1986,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>93</v>
       </c>
@@ -2002,7 +2006,7 @@
       </c>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>96</v>
       </c>
@@ -2020,7 +2024,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>98</v>
       </c>
@@ -2098,7 +2102,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>114</v>
       </c>
@@ -2118,7 +2122,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>119</v>
       </c>
@@ -2172,7 +2176,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>129</v>
       </c>
@@ -2192,7 +2196,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>134</v>
       </c>
@@ -2232,7 +2236,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>142</v>
       </c>
@@ -2250,7 +2254,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>146</v>
       </c>
@@ -2268,7 +2272,7 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>149</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>161</v>
       </c>
@@ -2408,7 +2412,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>176</v>
       </c>
@@ -2427,7 +2431,14 @@
       <c r="H46" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H46" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SimpleData"/>
+        <filter val="SimpleDataColumn"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3241,7 +3252,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,6 +3329,299 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422C86D5-5AE2-4AE7-8173-B2EAE1127368}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="6" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C12E4A-16B7-4BDB-A505-E9F8BECA4217}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="6" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B35207-89F8-4FE5-91A2-26FF876489B1}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="6" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>

</xml_diff>